<commit_message>
subida de la Rubica
</commit_message>
<xml_diff>
--- a/RúbricaDeEvaluación.xlsx
+++ b/RúbricaDeEvaluación.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jose\Documents\Universidad\8° Semestre\AREP\Talleres\Taller 1\AREP-Calculadora-estadistica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jose\Documents\Universidad\8° Semestre\AREP\Talleres\Taller 2\AREP-Calculadora-estadistica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1171BC5E-DCC0-4FB1-8C43-766CDC021B69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2485939-387F-4C5D-A9DA-E41C7632BC06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{30389B9F-C7D3-A542-9567-157FC0B6A65B}"/>
   </bookViews>
@@ -176,14 +176,14 @@
     <t>Juan Camilo Rojas Ortiz</t>
   </si>
   <si>
-    <t>https://github.com/Jcro15/AREP-taller1</t>
+    <t>https://github.com/Jcro15/Lab-SparkWeb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -209,6 +209,14 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -276,7 +284,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -295,6 +303,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -613,7 +622,7 @@
   <dimension ref="A2:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -630,7 +639,7 @@
         <v>36</v>
       </c>
       <c r="B3" s="11">
-        <v>44057</v>
+        <v>44064</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -639,7 +648,7 @@
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="14" t="s">
         <v>45</v>
       </c>
       <c r="C4" s="4"/>
@@ -1168,7 +1177,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{A0FAFCC5-1142-424A-87DB-A7840096E682}"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{8F8AAB44-17D9-4E41-8945-F2530B64C238}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>